<commit_message>
updated velpatasvir company code.
</commit_message>
<xml_diff>
--- a/tabular/drug_resistance/drugs.xlsx
+++ b/tabular/drug_resistance/drugs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Drug</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>velpatasvir</t>
+  </si>
+  <si>
+    <t>GS-5816</t>
   </si>
 </sst>
 </file>
@@ -157,8 +160,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -189,7 +194,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -202,6 +207,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -214,6 +220,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,7 +553,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A12" sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -670,6 +677,9 @@
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="16">
       <c r="A11" s="2" t="s">

</xml_diff>